<commit_message>
Ajouté différence fusible/porte fusible
</commit_message>
<xml_diff>
--- a/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
+++ b/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="215">
   <si>
     <t>Pos.</t>
   </si>
@@ -672,6 +672,12 @@
   </si>
   <si>
     <t>IsStocked</t>
+  </si>
+  <si>
+    <t>XF1</t>
+  </si>
+  <si>
+    <t>Fusible FST 2A temporisé</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1122,6 +1128,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1140,18 +1153,114 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1402,96 +1511,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1506,19 +1525,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:K54" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:K54" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A4:K54"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Pos." dataDxfId="32"/>
-    <tableColumn id="2" name="Designator" dataDxfId="31"/>
+    <tableColumn id="1" name="Pos." dataDxfId="8"/>
+    <tableColumn id="2" name="Designator" dataDxfId="7"/>
     <tableColumn id="3" name="Description"/>
-    <tableColumn id="4" name="PN" dataDxfId="30"/>
-    <tableColumn id="5" name="Quantity" dataDxfId="29"/>
-    <tableColumn id="6" name="Supplier 1" dataDxfId="28"/>
+    <tableColumn id="4" name="PN" dataDxfId="6"/>
+    <tableColumn id="5" name="Quantity" dataDxfId="5"/>
+    <tableColumn id="6" name="Supplier 1" dataDxfId="4"/>
     <tableColumn id="7" name="Supplier Part Number 1"/>
-    <tableColumn id="8" name="Supplier Price 1" dataDxfId="27"/>
-    <tableColumn id="9" name="Order Qty" dataDxfId="26"/>
-    <tableColumn id="10" name="Total" dataDxfId="25"/>
+    <tableColumn id="8" name="Supplier Price 1" dataDxfId="3"/>
+    <tableColumn id="9" name="Order Qty" dataDxfId="2"/>
+    <tableColumn id="10" name="Total" dataDxfId="1"/>
     <tableColumn id="11" name="IsStocked"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1793,8 +1812,8 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1817,64 +1836,64 @@
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="32" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="13"/>
-      <c r="H1" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="H1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="33" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="36" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -1913,7 +1932,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="26">
-        <f>ROW(A5) - ROW($A$4)</f>
+        <f t="shared" ref="A5:A36" si="0">ROW(A5) - ROW($A$4)</f>
         <v>1</v>
       </c>
       <c r="B5" s="30">
@@ -1951,7 +1970,7 @@
     </row>
     <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
-        <f>ROW(A6) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B6" s="31" t="s">
@@ -1976,7 +1995,7 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="I6" s="21">
-        <f t="shared" ref="I6:I53" si="0">$C$3*E6</f>
+        <f t="shared" ref="I6" si="1">$C$3*E6</f>
         <v>6</v>
       </c>
       <c r="J6" s="24">
@@ -1989,7 +2008,7 @@
     </row>
     <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
-        <f>ROW(A7) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" s="30" t="s">
@@ -2027,7 +2046,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
-        <f>ROW(A8) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B8" s="31" t="s">
@@ -2052,7 +2071,7 @@
         <v>1.23E-2</v>
       </c>
       <c r="I8" s="21">
-        <f t="shared" ref="I8" si="1">$C$3*E8</f>
+        <f t="shared" ref="I8" si="2">$C$3*E8</f>
         <v>1</v>
       </c>
       <c r="J8" s="24">
@@ -2065,7 +2084,7 @@
     </row>
     <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
-        <f>ROW(A9) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -2103,7 +2122,7 @@
     </row>
     <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
-        <f>ROW(A10) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B10" s="31" t="s">
@@ -2128,7 +2147,7 @@
         <v>4.57</v>
       </c>
       <c r="I10" s="21">
-        <f t="shared" ref="I10:I12" si="2">$C$3*E10</f>
+        <f t="shared" ref="I10" si="3">$C$3*E10</f>
         <v>2</v>
       </c>
       <c r="J10" s="24">
@@ -2141,29 +2160,29 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
-        <f>ROW(A11) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>124</v>
+        <v>214</v>
+      </c>
+      <c r="D11" s="45">
+        <v>261.476</v>
       </c>
       <c r="E11" s="28">
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>168</v>
+        <v>2</v>
       </c>
       <c r="G11" s="5">
-        <v>3517015</v>
+        <v>261.476</v>
       </c>
       <c r="H11" s="23">
-        <v>1.1100000000000001</v>
+        <v>0.33</v>
       </c>
       <c r="I11" s="20">
         <f>$C$3*E11</f>
@@ -2171,7 +2190,7 @@
       </c>
       <c r="J11" s="23">
         <f>H11*I11</f>
-        <v>1.1100000000000001</v>
+        <v>0.33</v>
       </c>
       <c r="K11" s="15" t="b">
         <v>1</v>
@@ -2179,7 +2198,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
-        <f>ROW(A12) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B12" s="31" t="s">
@@ -2204,7 +2223,7 @@
         <v>1.33</v>
       </c>
       <c r="I12" s="21">
-        <f t="shared" ref="I12" si="3">$C$3*E12</f>
+        <f t="shared" ref="I12" si="4">$C$3*E12</f>
         <v>2</v>
       </c>
       <c r="J12" s="24">
@@ -2217,7 +2236,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
-        <f>ROW(A13) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B13" s="30" t="s">
@@ -2255,7 +2274,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
-        <f>ROW(A14) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B14" s="31" t="s">
@@ -2280,7 +2299,7 @@
         <v>0.65800000000000003</v>
       </c>
       <c r="I14" s="21">
-        <f t="shared" ref="I14:I20" si="4">$C$3*E14</f>
+        <f t="shared" ref="I14" si="5">$C$3*E14</f>
         <v>1</v>
       </c>
       <c r="J14" s="24">
@@ -2293,7 +2312,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
-        <f>ROW(A15) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B15" s="30" t="s">
@@ -2331,7 +2350,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
-        <f>ROW(A16) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -2356,7 +2375,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="I16" s="21">
-        <f t="shared" ref="I16" si="5">$C$3*E16</f>
+        <f t="shared" ref="I16" si="6">$C$3*E16</f>
         <v>4</v>
       </c>
       <c r="J16" s="24">
@@ -2369,7 +2388,7 @@
     </row>
     <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
-        <f>ROW(A17) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
@@ -2407,7 +2426,7 @@
     </row>
     <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
-        <f>ROW(A18) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B18" s="31" t="s">
@@ -2432,7 +2451,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="I18" s="21">
-        <f t="shared" ref="I18:I20" si="6">$C$3*E18</f>
+        <f t="shared" ref="I18" si="7">$C$3*E18</f>
         <v>1</v>
       </c>
       <c r="J18" s="24">
@@ -2445,7 +2464,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
-        <f>ROW(A19) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B19" s="30" t="s">
@@ -2483,7 +2502,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
-        <f>ROW(A20) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B20" s="31" t="s">
@@ -2508,7 +2527,7 @@
         <v>0.02</v>
       </c>
       <c r="I20" s="21">
-        <f t="shared" ref="I20" si="7">$C$3*E20</f>
+        <f t="shared" ref="I20" si="8">$C$3*E20</f>
         <v>1</v>
       </c>
       <c r="J20" s="24">
@@ -2521,7 +2540,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
-        <f>ROW(A21) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B21" s="30" t="s">
@@ -2559,7 +2578,7 @@
     </row>
     <row r="22" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
-        <f>ROW(A22) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B22" s="31" t="s">
@@ -2584,7 +2603,7 @@
         <v>0.15</v>
       </c>
       <c r="I22" s="21">
-        <f t="shared" ref="I22:I36" si="8">$C$3*E22</f>
+        <f t="shared" ref="I22" si="9">$C$3*E22</f>
         <v>2</v>
       </c>
       <c r="J22" s="24">
@@ -2597,7 +2616,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
-        <f>ROW(A23) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -2635,7 +2654,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
-        <f>ROW(A24) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B24" s="31" t="s">
@@ -2660,7 +2679,7 @@
         <v>0.02</v>
       </c>
       <c r="I24" s="21">
-        <f t="shared" ref="I24" si="9">$C$3*E24</f>
+        <f t="shared" ref="I24" si="10">$C$3*E24</f>
         <v>2</v>
       </c>
       <c r="J24" s="24">
@@ -2673,7 +2692,7 @@
     </row>
     <row r="25" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
-        <f>ROW(A25) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B25" s="30" t="s">
@@ -2711,7 +2730,7 @@
     </row>
     <row r="26" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
-        <f>ROW(A26) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -2736,7 +2755,7 @@
         <v>0.02</v>
       </c>
       <c r="I26" s="21">
-        <f t="shared" ref="I26:I28" si="10">$C$3*E26</f>
+        <f t="shared" ref="I26" si="11">$C$3*E26</f>
         <v>4</v>
       </c>
       <c r="J26" s="24">
@@ -2749,7 +2768,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
-        <f>ROW(A27) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B27" s="30" t="s">
@@ -2787,7 +2806,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
-        <f>ROW(A28) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B28" s="31" t="s">
@@ -2812,7 +2831,7 @@
         <v>0.02</v>
       </c>
       <c r="I28" s="21">
-        <f t="shared" ref="I28" si="11">$C$3*E28</f>
+        <f t="shared" ref="I28" si="12">$C$3*E28</f>
         <v>2</v>
       </c>
       <c r="J28" s="24">
@@ -2825,7 +2844,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
-        <f>ROW(A29) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B29" s="30" t="s">
@@ -2863,7 +2882,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
-        <f>ROW(A30) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B30" s="31" t="s">
@@ -2888,7 +2907,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="I30" s="21">
-        <f t="shared" ref="I30:I36" si="12">$C$3*E30</f>
+        <f t="shared" ref="I30" si="13">$C$3*E30</f>
         <v>3</v>
       </c>
       <c r="J30" s="24">
@@ -2901,7 +2920,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
-        <f>ROW(A31) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B31" s="30" t="s">
@@ -2939,7 +2958,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
-        <f>ROW(A32) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B32" s="31" t="s">
@@ -2964,7 +2983,7 @@
         <v>0.02</v>
       </c>
       <c r="I32" s="21">
-        <f t="shared" ref="I32" si="13">$C$3*E32</f>
+        <f t="shared" ref="I32" si="14">$C$3*E32</f>
         <v>2</v>
       </c>
       <c r="J32" s="24">
@@ -2977,7 +2996,7 @@
     </row>
     <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
-        <f>ROW(A33) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B33" s="30" t="s">
@@ -3015,7 +3034,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
-        <f>ROW(A34) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B34" s="31" t="s">
@@ -3040,7 +3059,7 @@
         <v>0.02</v>
       </c>
       <c r="I34" s="21">
-        <f t="shared" ref="I34:I36" si="14">$C$3*E34</f>
+        <f t="shared" ref="I34" si="15">$C$3*E34</f>
         <v>1</v>
       </c>
       <c r="J34" s="24">
@@ -3053,7 +3072,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
-        <f>ROW(A35) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B35" s="30" t="s">
@@ -3091,7 +3110,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="27">
-        <f>ROW(A36) - ROW($A$4)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -3116,7 +3135,7 @@
         <v>2.12</v>
       </c>
       <c r="I36" s="21">
-        <f t="shared" ref="I36" si="15">$C$3*E36</f>
+        <f t="shared" ref="I36" si="16">$C$3*E36</f>
         <v>1</v>
       </c>
       <c r="J36" s="24">
@@ -3129,7 +3148,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
-        <f>ROW(A37) - ROW($A$4)</f>
+        <f t="shared" ref="A37:A54" si="17">ROW(A37) - ROW($A$4)</f>
         <v>33</v>
       </c>
       <c r="B37" s="30" t="s">
@@ -3167,7 +3186,7 @@
     </row>
     <row r="38" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="27">
-        <f>ROW(A38) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>34</v>
       </c>
       <c r="B38" s="31" t="s">
@@ -3192,7 +3211,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="I38" s="21">
-        <f t="shared" ref="I38:I53" si="16">$C$3*E38</f>
+        <f t="shared" ref="I38" si="18">$C$3*E38</f>
         <v>1</v>
       </c>
       <c r="J38" s="24">
@@ -3203,7 +3222,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
-        <f>ROW(A39) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>35</v>
       </c>
       <c r="B39" s="30" t="s">
@@ -3241,7 +3260,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="27">
-        <f>ROW(A40) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>36</v>
       </c>
       <c r="B40" s="31" t="s">
@@ -3266,7 +3285,7 @@
         <v>0.02</v>
       </c>
       <c r="I40" s="21">
-        <f t="shared" ref="I40" si="17">$C$3*E40</f>
+        <f t="shared" ref="I40" si="19">$C$3*E40</f>
         <v>1</v>
       </c>
       <c r="J40" s="24">
@@ -3279,7 +3298,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="26">
-        <f>ROW(A41) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>37</v>
       </c>
       <c r="B41" s="30" t="s">
@@ -3317,7 +3336,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="27">
-        <f>ROW(A42) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>38</v>
       </c>
       <c r="B42" s="31" t="s">
@@ -3342,7 +3361,7 @@
         <v>0.02</v>
       </c>
       <c r="I42" s="21">
-        <f t="shared" ref="I42:I44" si="18">$C$3*E42</f>
+        <f t="shared" ref="I42" si="20">$C$3*E42</f>
         <v>2</v>
       </c>
       <c r="J42" s="24">
@@ -3355,7 +3374,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="26">
-        <f>ROW(A43) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>39</v>
       </c>
       <c r="B43" s="30" t="s">
@@ -3393,7 +3412,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="27">
-        <f>ROW(A44) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>40</v>
       </c>
       <c r="B44" s="31" t="s">
@@ -3418,7 +3437,7 @@
         <v>0.02</v>
       </c>
       <c r="I44" s="21">
-        <f t="shared" ref="I44" si="19">$C$3*E44</f>
+        <f t="shared" ref="I44" si="21">$C$3*E44</f>
         <v>1</v>
       </c>
       <c r="J44" s="24">
@@ -3431,7 +3450,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="26">
-        <f>ROW(A45) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>41</v>
       </c>
       <c r="B45" s="30" t="s">
@@ -3469,7 +3488,7 @@
     </row>
     <row r="46" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="27">
-        <f>ROW(A46) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>42</v>
       </c>
       <c r="B46" s="31" t="s">
@@ -3494,7 +3513,7 @@
         <v>12.83</v>
       </c>
       <c r="I46" s="21">
-        <f t="shared" ref="I46:I52" si="20">$C$3*E46</f>
+        <f t="shared" ref="I46" si="22">$C$3*E46</f>
         <v>1</v>
       </c>
       <c r="J46" s="24">
@@ -3507,7 +3526,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="26">
-        <f>ROW(A47) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>43</v>
       </c>
       <c r="B47" s="30" t="s">
@@ -3545,7 +3564,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="27">
-        <f>ROW(A48) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>44</v>
       </c>
       <c r="B48" s="31" t="s">
@@ -3570,7 +3589,7 @@
         <v>1.51</v>
       </c>
       <c r="I48" s="21">
-        <f t="shared" ref="I48" si="21">$C$3*E48</f>
+        <f t="shared" ref="I48" si="23">$C$3*E48</f>
         <v>1</v>
       </c>
       <c r="J48" s="24">
@@ -3583,7 +3602,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="26">
-        <f>ROW(A49) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>45</v>
       </c>
       <c r="B49" s="30" t="s">
@@ -3621,7 +3640,7 @@
     </row>
     <row r="50" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="27">
-        <f>ROW(A50) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>46</v>
       </c>
       <c r="B50" s="31" t="s">
@@ -3646,7 +3665,7 @@
         <v>0.29310000000000003</v>
       </c>
       <c r="I50" s="21">
-        <f t="shared" ref="I50:I52" si="22">$C$3*E50</f>
+        <f t="shared" ref="I50" si="24">$C$3*E50</f>
         <v>8</v>
       </c>
       <c r="J50" s="24">
@@ -3659,7 +3678,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="26">
-        <f>ROW(A51) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>47</v>
       </c>
       <c r="B51" s="30" t="s">
@@ -3697,7 +3716,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="27">
-        <f>ROW(A52) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>48</v>
       </c>
       <c r="B52" s="31" t="s">
@@ -3714,7 +3733,7 @@
       <c r="G52" s="8"/>
       <c r="H52" s="24"/>
       <c r="I52" s="21">
-        <f t="shared" ref="I52" si="23">$C$3*E52</f>
+        <f t="shared" ref="I52" si="25">$C$3*E52</f>
         <v>2</v>
       </c>
       <c r="J52" s="24">
@@ -3725,7 +3744,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="26">
-        <f>ROW(A53) - ROW($A$4)</f>
+        <f t="shared" si="17"/>
         <v>49</v>
       </c>
       <c r="B53" s="30" t="s">
@@ -3762,17 +3781,42 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="15"/>
+      <c r="A54" s="26">
+        <f t="shared" si="17"/>
+        <v>50</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E54" s="28">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="5">
+        <v>3517015</v>
+      </c>
+      <c r="H54" s="23">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I54" s="20">
+        <f>$C$3*E54</f>
+        <v>1</v>
+      </c>
+      <c r="J54" s="23">
+        <f>H54*I54</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K54" s="15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H55" s="11" t="s">
@@ -3784,7 +3828,7 @@
       </c>
       <c r="J55" s="25">
         <f>SUM(J5:J53)</f>
-        <v>60.905100000000019</v>
+        <v>60.125100000000018</v>
       </c>
     </row>
   </sheetData>
@@ -3802,7 +3846,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{64211BAB-4930-4668-885C-0EA0CE6E5BE5}">
+          <x14:cfRule type="containsText" priority="26" operator="containsText" id="{64211BAB-4930-4668-885C-0EA0CE6E5BE5}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K5)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3816,10 +3860,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>K5:K6 K54</xm:sqref>
+          <xm:sqref>K5:K6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{6FBE027B-FB31-47A7-ACD4-5ED830F01C76}">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{6FBE027B-FB31-47A7-ACD4-5ED830F01C76}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K7)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3836,7 +3880,7 @@
           <xm:sqref>K7:K8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{D6737FEC-398A-4950-AAC9-87E32874816F}">
+          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{D6737FEC-398A-4950-AAC9-87E32874816F}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K9)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3853,7 +3897,7 @@
           <xm:sqref>K9:K10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{F9B55B37-24E8-46AF-93D6-51E983D4D7FB}">
+          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{F9B55B37-24E8-46AF-93D6-51E983D4D7FB}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K11)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3870,7 +3914,7 @@
           <xm:sqref>K11:K12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{A99328FB-6DD2-4FAE-A5AC-FF5361A896DC}">
+          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{A99328FB-6DD2-4FAE-A5AC-FF5361A896DC}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K13)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3887,7 +3931,7 @@
           <xm:sqref>K13:K14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{CF425ADF-23AF-4D01-A856-26B837E66F20}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{CF425ADF-23AF-4D01-A856-26B837E66F20}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K15)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3904,7 +3948,7 @@
           <xm:sqref>K15:K16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{FDF292FD-2556-4C43-988B-4E606602AE1A}">
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{FDF292FD-2556-4C43-988B-4E606602AE1A}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K17)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3921,7 +3965,7 @@
           <xm:sqref>K17:K18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{B8FDC38D-7798-4160-B79D-C22876C4C4C8}">
+          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{B8FDC38D-7798-4160-B79D-C22876C4C4C8}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K19)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3938,7 +3982,7 @@
           <xm:sqref>K19:K20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{7AFFE315-B12C-45DD-9BDD-7C8FF009D0DE}">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{7AFFE315-B12C-45DD-9BDD-7C8FF009D0DE}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K21)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3955,7 +3999,7 @@
           <xm:sqref>K21:K22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{E8FCE739-FFF1-40CE-BCAB-2D651A3BADB1}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{E8FCE739-FFF1-40CE-BCAB-2D651A3BADB1}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K23)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3972,7 +4016,7 @@
           <xm:sqref>K23:K24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{C24429B6-1BA3-4EAE-B100-0017F99253EE}">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{C24429B6-1BA3-4EAE-B100-0017F99253EE}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K25)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3989,7 +4033,7 @@
           <xm:sqref>K25:K26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{48D25579-98DB-4EB8-B317-44852011B7BF}">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{48D25579-98DB-4EB8-B317-44852011B7BF}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K27)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4006,7 +4050,7 @@
           <xm:sqref>K27:K28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{4CF3A302-41E6-4941-B446-820644F9FB81}">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{4CF3A302-41E6-4941-B446-820644F9FB81}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K29)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4023,7 +4067,7 @@
           <xm:sqref>K29:K30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{0EA78D8C-0397-415F-A73F-A9A5C6DF7E55}">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{0EA78D8C-0397-415F-A73F-A9A5C6DF7E55}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K31)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4040,7 +4084,7 @@
           <xm:sqref>K31:K32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{7F32302F-4857-434D-AEA3-81391C5C59B1}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{7F32302F-4857-434D-AEA3-81391C5C59B1}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K33)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4057,7 +4101,7 @@
           <xm:sqref>K33:K34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{E915A3BD-8CFA-4BBB-BBCE-F009A57E2765}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{E915A3BD-8CFA-4BBB-BBCE-F009A57E2765}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K35)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4074,7 +4118,7 @@
           <xm:sqref>K35:K36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{D7309C52-80A0-42D9-A575-494A967FB4F3}">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{D7309C52-80A0-42D9-A575-494A967FB4F3}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K37)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4091,7 +4135,7 @@
           <xm:sqref>K37:K38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{F7C80090-A7B1-4281-8B29-E9ABEC36FF97}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{F7C80090-A7B1-4281-8B29-E9ABEC36FF97}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K39)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4108,7 +4152,7 @@
           <xm:sqref>K39:K40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{59F87D3C-147F-42C5-93FB-B90260368DCA}">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{59F87D3C-147F-42C5-93FB-B90260368DCA}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K41)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4125,7 +4169,7 @@
           <xm:sqref>K41:K42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{BBA637B9-0EF5-4AA2-A01B-2139D5C19B85}">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{BBA637B9-0EF5-4AA2-A01B-2139D5C19B85}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K43)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4142,7 +4186,7 @@
           <xm:sqref>K43:K44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{FFE59934-756D-49E5-8C7D-28BA6CA91EB4}">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{FFE59934-756D-49E5-8C7D-28BA6CA91EB4}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K45)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4159,7 +4203,7 @@
           <xm:sqref>K45:K46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{ED4D6400-4655-4260-9F29-A7F61CAE3E29}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{ED4D6400-4655-4260-9F29-A7F61CAE3E29}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K47)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4176,7 +4220,7 @@
           <xm:sqref>K47:K48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{745AC6A4-0C3F-478C-AAB0-E6FC83B60CE9}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{745AC6A4-0C3F-478C-AAB0-E6FC83B60CE9}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K49)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4193,7 +4237,7 @@
           <xm:sqref>K49:K50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{821DEDD2-C95D-4A36-8049-3A6332ACFDDF}">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{821DEDD2-C95D-4A36-8049-3A6332ACFDDF}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K51)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4210,7 +4254,7 @@
           <xm:sqref>K51:K52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{C3DEA72A-D2C1-45A6-97B4-7001AA369A16}">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{C3DEA72A-D2C1-45A6-97B4-7001AA369A16}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K53)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4225,6 +4269,23 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>K53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{1B409C2E-0B48-494C-ABA1-9D5126DC6A07}">
+            <xm:f>NOT(ISERROR(SEARCH("VRAI",K54)))</xm:f>
+            <xm:f>"VRAI"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>K54</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4244,15 +4305,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4f37139f2ce50ec3ac02e3d1ccd0c1ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xmlns:ns3="98d92101-24da-4498-9971-a24673344bd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91fee7e25855f2cb58de83858d7f3967" ns2:_="" ns3:_="">
     <xsd:import namespace="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
@@ -4487,32 +4539,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A056176-9FE1-4C5F-A929-245972C77676}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
-    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5456B884-6AB4-45D3-8FD2-E75BD30FD293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2CADE7-C340-4D0B-BD99-05BB04C9DCF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4529,4 +4582,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5456B884-6AB4-45D3-8FD2-E75BD30FD293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Réception des produits Mouser
</commit_message>
<xml_diff>
--- a/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
+++ b/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud.sharepoint.com/sites/ETML_FLO-22-24_Teams/Documents partages/Partages/Vasseur/DAT/1438/5-Hardware/1438-5100-Puit de courant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyvasseur\Education Vaud\ETML_FLO-22-24_Teams - Vasseur\DAT\1438\5-Hardware\1438-5100-Puit de courant\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="216">
   <si>
     <t>Pos.</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t>Fusible FST 2A temporisé</t>
+  </si>
+  <si>
+    <t>Reçu</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -732,6 +735,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1043,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1135,6 +1143,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1153,24 +1167,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="38">
     <dxf>
       <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     </dxf>
@@ -1511,6 +1512,26 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1525,20 +1546,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:K54" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A4:K54"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="Pos." dataDxfId="8"/>
-    <tableColumn id="2" name="Designator" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:L54" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A4:L54">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="ETML"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Pos." dataDxfId="7"/>
+    <tableColumn id="2" name="Designator" dataDxfId="6"/>
     <tableColumn id="3" name="Description"/>
-    <tableColumn id="4" name="PN" dataDxfId="6"/>
-    <tableColumn id="5" name="Quantity" dataDxfId="5"/>
-    <tableColumn id="6" name="Supplier 1" dataDxfId="4"/>
+    <tableColumn id="4" name="PN" dataDxfId="5"/>
+    <tableColumn id="5" name="Quantity" dataDxfId="4"/>
+    <tableColumn id="6" name="Supplier 1" dataDxfId="3"/>
     <tableColumn id="7" name="Supplier Part Number 1"/>
-    <tableColumn id="8" name="Supplier Price 1" dataDxfId="3"/>
-    <tableColumn id="9" name="Order Qty" dataDxfId="2"/>
-    <tableColumn id="10" name="Total" dataDxfId="1"/>
+    <tableColumn id="8" name="Supplier Price 1" dataDxfId="2"/>
+    <tableColumn id="9" name="Order Qty" dataDxfId="1"/>
+    <tableColumn id="10" name="Total" dataDxfId="0"/>
     <tableColumn id="11" name="IsStocked"/>
+    <tableColumn id="12" name="Reçu"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1810,10 +1838,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1832,7 +1860,7 @@
     <col min="12" max="256" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1847,13 +1875,13 @@
         <v>12</v>
       </c>
       <c r="G1" s="13"/>
-      <c r="H1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="41"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1870,11 +1898,11 @@
       <c r="G2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1891,11 +1919,11 @@
       <c r="G3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
-    </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+    </row>
+    <row r="4" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
@@ -1929,8 +1957,11 @@
       <c r="K4" s="19" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="40" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26">
         <f t="shared" ref="A5:A36" si="0">ROW(A5) - ROW($A$4)</f>
         <v>1</v>
@@ -1968,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2005,8 +2036,11 @@
       <c r="K6" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2043,8 +2077,11 @@
       <c r="K7" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2081,8 +2118,11 @@
       <c r="K8" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2119,8 +2159,11 @@
       <c r="K9" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2157,8 +2200,11 @@
       <c r="K10" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2169,7 +2215,7 @@
       <c r="C11" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="39">
         <v>261.476</v>
       </c>
       <c r="E11" s="28">
@@ -2195,8 +2241,11 @@
       <c r="K11" s="15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2233,8 +2282,11 @@
       <c r="K12" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2271,8 +2323,11 @@
       <c r="K13" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2309,8 +2364,11 @@
       <c r="K14" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2347,8 +2405,11 @@
       <c r="K15" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2385,8 +2446,11 @@
       <c r="K16" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2424,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2461,8 +2525,11 @@
       <c r="K18" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2500,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2537,8 +2604,11 @@
       <c r="K20" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2576,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2614,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2651,8 +2721,11 @@
       <c r="K23" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2689,8 +2762,11 @@
       <c r="K24" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2728,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2765,8 +2841,11 @@
       <c r="K26" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2803,8 +2882,11 @@
       <c r="K27" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2841,8 +2923,11 @@
       <c r="K28" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2879,8 +2964,11 @@
       <c r="K29" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2917,8 +3005,11 @@
       <c r="K30" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2955,8 +3046,11 @@
       <c r="K31" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2993,8 +3087,11 @@
       <c r="K32" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3031,8 +3128,11 @@
       <c r="K33" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3069,8 +3169,11 @@
       <c r="K34" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3107,8 +3210,11 @@
       <c r="K35" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3145,8 +3251,11 @@
       <c r="K36" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
         <f t="shared" ref="A37:A54" si="17">ROW(A37) - ROW($A$4)</f>
         <v>33</v>
@@ -3183,8 +3292,11 @@
       <c r="K37" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="27">
         <f t="shared" si="17"/>
         <v>34</v>
@@ -3219,8 +3331,11 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="K38" s="16"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
         <f t="shared" si="17"/>
         <v>35</v>
@@ -3257,8 +3372,11 @@
       <c r="K39" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="27">
         <f t="shared" si="17"/>
         <v>36</v>
@@ -3295,8 +3413,11 @@
       <c r="K40" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="26">
         <f t="shared" si="17"/>
         <v>37</v>
@@ -3333,8 +3454,11 @@
       <c r="K41" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="27">
         <f t="shared" si="17"/>
         <v>38</v>
@@ -3371,8 +3495,11 @@
       <c r="K42" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="26">
         <f t="shared" si="17"/>
         <v>39</v>
@@ -3409,8 +3536,11 @@
       <c r="K43" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="27">
         <f t="shared" si="17"/>
         <v>40</v>
@@ -3447,8 +3577,11 @@
       <c r="K44" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="26">
         <f t="shared" si="17"/>
         <v>41</v>
@@ -3485,8 +3618,11 @@
       <c r="K45" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="27">
         <f t="shared" si="17"/>
         <v>42</v>
@@ -3523,8 +3659,11 @@
       <c r="K46" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="26">
         <f t="shared" si="17"/>
         <v>43</v>
@@ -3561,8 +3700,11 @@
       <c r="K47" s="15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="27">
         <f t="shared" si="17"/>
         <v>44</v>
@@ -3599,8 +3741,11 @@
       <c r="K48" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="26">
         <f t="shared" si="17"/>
         <v>45</v>
@@ -3637,8 +3782,11 @@
       <c r="K49" s="15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="27">
         <f t="shared" si="17"/>
         <v>46</v>
@@ -3675,8 +3823,11 @@
       <c r="K50" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="26">
         <f t="shared" si="17"/>
         <v>47</v>
@@ -3713,8 +3864,11 @@
       <c r="K51" s="15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="27">
         <f t="shared" si="17"/>
         <v>48</v>
@@ -3742,7 +3896,7 @@
       </c>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="26">
         <f t="shared" si="17"/>
         <v>49</v>
@@ -3779,8 +3933,11 @@
       <c r="K53" s="15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26">
         <f t="shared" si="17"/>
         <v>50</v>
@@ -3818,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H55" s="11" t="s">
         <v>8</v>
       </c>
@@ -3836,6 +3993,11 @@
     <mergeCell ref="H1:J3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -3846,7 +4008,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="26" operator="containsText" id="{64211BAB-4930-4668-885C-0EA0CE6E5BE5}">
+          <x14:cfRule type="containsText" priority="27" operator="containsText" id="{64211BAB-4930-4668-885C-0EA0CE6E5BE5}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K5)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3863,7 +4025,7 @@
           <xm:sqref>K5:K6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{6FBE027B-FB31-47A7-ACD4-5ED830F01C76}">
+          <x14:cfRule type="containsText" priority="26" operator="containsText" id="{6FBE027B-FB31-47A7-ACD4-5ED830F01C76}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K7)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3880,7 +4042,7 @@
           <xm:sqref>K7:K8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{D6737FEC-398A-4950-AAC9-87E32874816F}">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{D6737FEC-398A-4950-AAC9-87E32874816F}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K9)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3897,7 +4059,7 @@
           <xm:sqref>K9:K10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{F9B55B37-24E8-46AF-93D6-51E983D4D7FB}">
+          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{F9B55B37-24E8-46AF-93D6-51E983D4D7FB}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K11)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3914,7 +4076,7 @@
           <xm:sqref>K11:K12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{A99328FB-6DD2-4FAE-A5AC-FF5361A896DC}">
+          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{A99328FB-6DD2-4FAE-A5AC-FF5361A896DC}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K13)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3931,7 +4093,7 @@
           <xm:sqref>K13:K14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{CF425ADF-23AF-4D01-A856-26B837E66F20}">
+          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{CF425ADF-23AF-4D01-A856-26B837E66F20}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K15)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3948,7 +4110,7 @@
           <xm:sqref>K15:K16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{FDF292FD-2556-4C43-988B-4E606602AE1A}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{FDF292FD-2556-4C43-988B-4E606602AE1A}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K17)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3965,7 +4127,7 @@
           <xm:sqref>K17:K18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{B8FDC38D-7798-4160-B79D-C22876C4C4C8}">
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{B8FDC38D-7798-4160-B79D-C22876C4C4C8}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K19)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3982,7 +4144,7 @@
           <xm:sqref>K19:K20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{7AFFE315-B12C-45DD-9BDD-7C8FF009D0DE}">
+          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{7AFFE315-B12C-45DD-9BDD-7C8FF009D0DE}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K21)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3999,7 +4161,7 @@
           <xm:sqref>K21:K22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{E8FCE739-FFF1-40CE-BCAB-2D651A3BADB1}">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{E8FCE739-FFF1-40CE-BCAB-2D651A3BADB1}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K23)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4016,7 +4178,7 @@
           <xm:sqref>K23:K24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{C24429B6-1BA3-4EAE-B100-0017F99253EE}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{C24429B6-1BA3-4EAE-B100-0017F99253EE}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K25)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4033,7 +4195,7 @@
           <xm:sqref>K25:K26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{48D25579-98DB-4EB8-B317-44852011B7BF}">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{48D25579-98DB-4EB8-B317-44852011B7BF}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K27)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4050,7 +4212,7 @@
           <xm:sqref>K27:K28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{4CF3A302-41E6-4941-B446-820644F9FB81}">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{4CF3A302-41E6-4941-B446-820644F9FB81}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K29)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4067,7 +4229,7 @@
           <xm:sqref>K29:K30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{0EA78D8C-0397-415F-A73F-A9A5C6DF7E55}">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{0EA78D8C-0397-415F-A73F-A9A5C6DF7E55}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K31)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4084,7 +4246,7 @@
           <xm:sqref>K31:K32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{7F32302F-4857-434D-AEA3-81391C5C59B1}">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{7F32302F-4857-434D-AEA3-81391C5C59B1}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K33)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4101,7 +4263,7 @@
           <xm:sqref>K33:K34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{E915A3BD-8CFA-4BBB-BBCE-F009A57E2765}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{E915A3BD-8CFA-4BBB-BBCE-F009A57E2765}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K35)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4118,7 +4280,7 @@
           <xm:sqref>K35:K36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{D7309C52-80A0-42D9-A575-494A967FB4F3}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{D7309C52-80A0-42D9-A575-494A967FB4F3}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K37)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4135,7 +4297,7 @@
           <xm:sqref>K37:K38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{F7C80090-A7B1-4281-8B29-E9ABEC36FF97}">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{F7C80090-A7B1-4281-8B29-E9ABEC36FF97}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K39)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4152,7 +4314,7 @@
           <xm:sqref>K39:K40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{59F87D3C-147F-42C5-93FB-B90260368DCA}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{59F87D3C-147F-42C5-93FB-B90260368DCA}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K41)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4169,7 +4331,7 @@
           <xm:sqref>K41:K42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{BBA637B9-0EF5-4AA2-A01B-2139D5C19B85}">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{BBA637B9-0EF5-4AA2-A01B-2139D5C19B85}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K43)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4186,7 +4348,7 @@
           <xm:sqref>K43:K44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{FFE59934-756D-49E5-8C7D-28BA6CA91EB4}">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{FFE59934-756D-49E5-8C7D-28BA6CA91EB4}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K45)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4203,7 +4365,7 @@
           <xm:sqref>K45:K46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{ED4D6400-4655-4260-9F29-A7F61CAE3E29}">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{ED4D6400-4655-4260-9F29-A7F61CAE3E29}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K47)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4220,7 +4382,7 @@
           <xm:sqref>K47:K48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{745AC6A4-0C3F-478C-AAB0-E6FC83B60CE9}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{745AC6A4-0C3F-478C-AAB0-E6FC83B60CE9}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K49)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4237,7 +4399,7 @@
           <xm:sqref>K49:K50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{821DEDD2-C95D-4A36-8049-3A6332ACFDDF}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{821DEDD2-C95D-4A36-8049-3A6332ACFDDF}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K51)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4254,7 +4416,7 @@
           <xm:sqref>K51:K52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{C3DEA72A-D2C1-45A6-97B4-7001AA369A16}">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{C3DEA72A-D2C1-45A6-97B4-7001AA369A16}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K53)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4271,7 +4433,7 @@
           <xm:sqref>K53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{1B409C2E-0B48-494C-ABA1-9D5126DC6A07}">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{1B409C2E-0B48-494C-ABA1-9D5126DC6A07}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K54)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -4553,11 +4715,11 @@
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>

</xml_diff>

<commit_message>
Réception des produits Farnell
</commit_message>
<xml_diff>
--- a/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
+++ b/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
@@ -1550,7 +1550,7 @@
   <autoFilter ref="A4:L54">
     <filterColumn colId="5">
       <filters>
-        <filter val="ETML"/>
+        <filter val="Farnell"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1840,8 +1840,8 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2204,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2450,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2485,6 +2485,9 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="K17" s="15">
+        <v>1</v>
+      </c>
+      <c r="L17">
         <v>1</v>
       </c>
     </row>
@@ -2567,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2608,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2646,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2683,8 +2686,11 @@
       <c r="K22" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2725,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2766,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2803,8 +2809,11 @@
       <c r="K25" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2845,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2886,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2927,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3009,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3050,7 +3059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3132,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3173,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3255,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
         <f t="shared" ref="A37:A54" si="17">ROW(A37) - ROW($A$4)</f>
         <v>33</v>
@@ -3335,7 +3344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
         <f t="shared" si="17"/>
         <v>35</v>
@@ -3376,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="27">
         <f t="shared" si="17"/>
         <v>36</v>
@@ -3417,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="26">
         <f t="shared" si="17"/>
         <v>37</v>
@@ -3458,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="27">
         <f t="shared" si="17"/>
         <v>38</v>
@@ -3499,7 +3508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="26">
         <f t="shared" si="17"/>
         <v>39</v>
@@ -3540,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="27">
         <f t="shared" si="17"/>
         <v>40</v>
@@ -3581,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="26">
         <f t="shared" si="17"/>
         <v>41</v>
@@ -3622,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="27">
         <f t="shared" si="17"/>
         <v>42</v>
@@ -3663,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="26">
         <f t="shared" si="17"/>
         <v>43</v>
@@ -3704,7 +3713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="27">
         <f t="shared" si="17"/>
         <v>44</v>
@@ -3745,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="26">
         <f t="shared" si="17"/>
         <v>45</v>
@@ -3786,7 +3795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="27">
         <f t="shared" si="17"/>
         <v>46</v>
@@ -3827,7 +3836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="26">
         <f t="shared" si="17"/>
         <v>47</v>
@@ -3896,7 +3905,7 @@
       </c>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="26">
         <f t="shared" si="17"/>
         <v>49</v>
@@ -3937,7 +3946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26">
         <f t="shared" si="17"/>
         <v>50</v>
@@ -3972,6 +3981,9 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="K54" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L54">
         <v>1</v>
       </c>
     </row>
@@ -4467,6 +4479,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4f37139f2ce50ec3ac02e3d1ccd0c1ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xmlns:ns3="98d92101-24da-4498-9971-a24673344bd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91fee7e25855f2cb58de83858d7f3967" ns2:_="" ns3:_="">
     <xsd:import namespace="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
@@ -4701,33 +4722,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A056176-9FE1-4C5F-A929-245972C77676}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5456B884-6AB4-45D3-8FD2-E75BD30FD293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2CADE7-C340-4D0B-BD99-05BB04C9DCF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4744,12 +4764,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5456B884-6AB4-45D3-8FD2-E75BD30FD293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rasemblé symboles dans une librairie, début footprint TO220+cooler
</commit_message>
<xml_diff>
--- a/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
+++ b/5-Hardware/1438-5100-Puit de courant/1438-5600-Puit de courant_BOM.xlsx
@@ -1547,13 +1547,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:L54" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A4:L54">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Farnell"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:L54"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Pos." dataDxfId="7"/>
     <tableColumn id="2" name="Designator" dataDxfId="6"/>
@@ -1840,8 +1834,8 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1961,7 +1955,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="26">
         <f t="shared" ref="A5:A36" si="0">ROW(A5) - ROW($A$4)</f>
         <v>1</v>
@@ -1999,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2040,7 +2034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2081,7 +2075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2122,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2163,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2204,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2245,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2286,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2327,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2368,7 +2362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2409,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2491,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2532,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2569,8 +2563,11 @@
       <c r="K19" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2690,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2731,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2813,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2854,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2895,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2936,7 +2933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2977,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3018,7 +3015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3059,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3100,7 +3097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3141,7 +3138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3182,7 +3179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3223,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="27">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3264,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
         <f t="shared" ref="A37:A54" si="17">ROW(A37) - ROW($A$4)</f>
         <v>33</v>
@@ -3305,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="27">
         <f t="shared" si="17"/>
         <v>34</v>
@@ -3344,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
         <f t="shared" si="17"/>
         <v>35</v>
@@ -3385,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="27">
         <f t="shared" si="17"/>
         <v>36</v>
@@ -3426,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="26">
         <f t="shared" si="17"/>
         <v>37</v>
@@ -3467,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="27">
         <f t="shared" si="17"/>
         <v>38</v>
@@ -3508,7 +3505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="26">
         <f t="shared" si="17"/>
         <v>39</v>
@@ -3549,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="27">
         <f t="shared" si="17"/>
         <v>40</v>
@@ -3590,7 +3587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="26">
         <f t="shared" si="17"/>
         <v>41</v>
@@ -3631,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="27">
         <f t="shared" si="17"/>
         <v>42</v>
@@ -3672,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="26">
         <f t="shared" si="17"/>
         <v>43</v>
@@ -3713,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="27">
         <f t="shared" si="17"/>
         <v>44</v>
@@ -3754,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="26">
         <f t="shared" si="17"/>
         <v>45</v>
@@ -3795,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="27">
         <f t="shared" si="17"/>
         <v>46</v>
@@ -3836,7 +3833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="26">
         <f t="shared" si="17"/>
         <v>47</v>
@@ -3877,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="27">
         <f t="shared" si="17"/>
         <v>48</v>
@@ -3905,7 +3902,7 @@
       </c>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="26">
         <f t="shared" si="17"/>
         <v>49</v>
@@ -4479,15 +4476,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4f37139f2ce50ec3ac02e3d1ccd0c1ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xmlns:ns3="98d92101-24da-4498-9971-a24673344bd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91fee7e25855f2cb58de83858d7f3967" ns2:_="" ns3:_="">
     <xsd:import namespace="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
@@ -4722,32 +4710,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A056176-9FE1-4C5F-A929-245972C77676}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5456B884-6AB4-45D3-8FD2-E75BD30FD293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2CADE7-C340-4D0B-BD99-05BB04C9DCF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4764,4 +4753,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5456B884-6AB4-45D3-8FD2-E75BD30FD293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>